<commit_message>
Added temp, pH and larval collection data files
</commit_message>
<xml_diff>
--- a/Data/2017-Larval-Collection-Data.xlsx
+++ b/Data/2017-Larval-Collection-Data.xlsx
@@ -7,7 +7,8 @@
     <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="15460" tabRatio="500"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Larval collection counts" sheetId="1" r:id="rId1"/>
+    <sheet name="Larval Counts - rearing bucket" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="140000" concurrentCalc="0"/>
   <extLst>
@@ -19,14 +20,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="37">
   <si>
     <t>Group</t>
   </si>
   <si>
-    <t># Larvae Spawned</t>
-  </si>
-  <si>
     <t>K-10 amb pH</t>
   </si>
   <si>
@@ -48,9 +46,6 @@
     <t>Larvae released 9 days post-segregation; cannot keep these larvae b/c their genitors are unknown</t>
   </si>
   <si>
-    <t>Total Volume (mL)</t>
-  </si>
-  <si>
     <t>Count A</t>
   </si>
   <si>
@@ -61,6 +56,81 @@
   </si>
   <si>
     <t>Vol. for count (mL)</t>
+  </si>
+  <si>
+    <t>HL-6 low pH</t>
+  </si>
+  <si>
+    <t>Larvae had been in static catchment bucket for ~24hrs; didn't look good</t>
+  </si>
+  <si>
+    <t>SN-10 amb pH B</t>
+  </si>
+  <si>
+    <t>SN-6 amb pH A</t>
+  </si>
+  <si>
+    <t>SN-10 low pH A</t>
+  </si>
+  <si>
+    <t>Very frothy catchment bucket!</t>
+  </si>
+  <si>
+    <t>Total Vol (mL)</t>
+  </si>
+  <si>
+    <t># Larvae Collected</t>
+  </si>
+  <si>
+    <t># Larvae added to bucket</t>
+  </si>
+  <si>
+    <t># Larvae found in bucket</t>
+  </si>
+  <si>
+    <t>Date</t>
+  </si>
+  <si>
+    <t>Survival rate</t>
+  </si>
+  <si>
+    <t>A1</t>
+  </si>
+  <si>
+    <t>B1</t>
+  </si>
+  <si>
+    <t>C1</t>
+  </si>
+  <si>
+    <t>SN-10 amb pH A</t>
+  </si>
+  <si>
+    <t>A2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C2 </t>
+  </si>
+  <si>
+    <t>D2</t>
+  </si>
+  <si>
+    <t>A3</t>
+  </si>
+  <si>
+    <t>B3</t>
+  </si>
+  <si>
+    <t>C3</t>
+  </si>
+  <si>
+    <t>Temporary rearing bucket</t>
+  </si>
+  <si>
+    <t xml:space="preserve">*Did not differentiate between live &amp; dead, but most appeared in tact </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
   </si>
 </sst>
 </file>
@@ -68,9 +138,16 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
-    <numFmt numFmtId="165" formatCode="0.000"/>
+    <numFmt numFmtId="164" formatCode="0.000"/>
   </numFmts>
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -119,39 +196,104 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="11">
+  <cellStyleXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="11" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="11">
+  <cellStyles count="42">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="13" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="15" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="17" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="19" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="21" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="23" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="25" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="27" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="29" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="31" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="33" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="35" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="37" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="39" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="41" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="12" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="14" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="16" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="18" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="20" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="22" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="24" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="26" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="28" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="30" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="32" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="34" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="36" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="38" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="40" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Percent" xfId="11" builtinId="5"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
@@ -482,57 +624,58 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J1048576"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+    <sheetView tabSelected="1" showRuler="0" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="J15" sqref="J15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.75"/>
   <cols>
-    <col min="1" max="2" width="16.1640625" customWidth="1"/>
-    <col min="3" max="3" width="22.33203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14" customWidth="1"/>
-    <col min="5" max="6" width="16.1640625" customWidth="1"/>
-    <col min="7" max="7" width="21.6640625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="17.5" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="22.5" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="30.5" customWidth="1"/>
+    <col min="2" max="2" width="10.5" customWidth="1"/>
+    <col min="3" max="3" width="13.1640625" customWidth="1"/>
+    <col min="4" max="4" width="9.1640625" customWidth="1"/>
+    <col min="5" max="6" width="8.33203125" customWidth="1"/>
+    <col min="7" max="7" width="14" customWidth="1"/>
+    <col min="8" max="8" width="12.6640625" customWidth="1"/>
+    <col min="9" max="9" width="26.33203125" customWidth="1"/>
     <col min="10" max="10" width="98.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" s="5" customFormat="1" ht="29" customHeight="1">
+    <row r="1" spans="1:10" s="5" customFormat="1" ht="46" customHeight="1">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="E1" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="C1" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="D1" s="5" t="s">
+      <c r="F1" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="E1" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="F1" s="5" t="s">
-        <v>12</v>
-      </c>
       <c r="G1" s="5" t="s">
-        <v>1</v>
+        <v>19</v>
       </c>
       <c r="H1" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="I1" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="I1" s="5" t="s">
-        <v>5</v>
-      </c>
       <c r="J1" s="5" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="2" spans="1:10">
       <c r="A2" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B2">
         <v>300</v>
@@ -557,15 +700,15 @@
         <v>42866</v>
       </c>
       <c r="I2" t="s">
-        <v>6</v>
+        <v>34</v>
       </c>
       <c r="J2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="3" spans="1:10">
       <c r="A3" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B3">
         <v>300</v>
@@ -590,70 +733,316 @@
         <v>42866</v>
       </c>
       <c r="I3" t="s">
-        <v>6</v>
+        <v>34</v>
       </c>
       <c r="J3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="4" spans="1:10">
-      <c r="G4" s="1" t="e">
+      <c r="A4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B4">
+        <v>50</v>
+      </c>
+      <c r="C4">
+        <v>1</v>
+      </c>
+      <c r="D4">
+        <v>78</v>
+      </c>
+      <c r="E4">
+        <v>65</v>
+      </c>
+      <c r="F4">
+        <v>66</v>
+      </c>
+      <c r="G4" s="1">
         <f t="shared" ref="G4:G32" si="0">(AVERAGE(D4:F4)/C4)*B4</f>
-        <v>#DIV/0!</v>
+        <v>3483.3333333333335</v>
+      </c>
+      <c r="H4" s="2">
+        <v>42868</v>
+      </c>
+      <c r="I4" t="s">
+        <v>34</v>
+      </c>
+      <c r="J4" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="5" spans="1:10">
-      <c r="G5" s="1" t="e">
-        <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
+      <c r="A5" t="s">
+        <v>1</v>
+      </c>
+      <c r="B5">
+        <v>300</v>
+      </c>
+      <c r="C5">
+        <v>0.5</v>
+      </c>
+      <c r="D5">
+        <v>115</v>
+      </c>
+      <c r="E5">
+        <v>112</v>
+      </c>
+      <c r="F5">
+        <v>107</v>
+      </c>
+      <c r="G5" s="1">
+        <f t="shared" si="0"/>
+        <v>66800</v>
+      </c>
+      <c r="H5" s="2">
+        <v>42869</v>
+      </c>
+      <c r="I5" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="6" spans="1:10">
-      <c r="G6" s="1" t="e">
-        <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
+      <c r="A6" t="s">
+        <v>14</v>
+      </c>
+      <c r="B6">
+        <v>300</v>
+      </c>
+      <c r="C6">
+        <v>0.75</v>
+      </c>
+      <c r="D6">
+        <v>185</v>
+      </c>
+      <c r="E6">
+        <v>223</v>
+      </c>
+      <c r="F6">
+        <v>197</v>
+      </c>
+      <c r="G6" s="1">
+        <f t="shared" si="0"/>
+        <v>80666.666666666657</v>
+      </c>
+      <c r="H6" s="2">
+        <v>42869</v>
+      </c>
+      <c r="I6" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="7" spans="1:10">
-      <c r="G7" s="1" t="e">
-        <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
+      <c r="A7" t="s">
+        <v>15</v>
+      </c>
+      <c r="B7">
+        <v>300</v>
+      </c>
+      <c r="C7">
+        <v>0.75</v>
+      </c>
+      <c r="D7">
+        <v>173</v>
+      </c>
+      <c r="E7">
+        <v>175</v>
+      </c>
+      <c r="F7">
+        <v>170</v>
+      </c>
+      <c r="G7" s="1">
+        <f t="shared" si="0"/>
+        <v>69066.666666666657</v>
+      </c>
+      <c r="H7" s="2">
+        <v>42869</v>
+      </c>
+      <c r="I7" t="s">
+        <v>34</v>
+      </c>
+      <c r="J7" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="8" spans="1:10">
-      <c r="G8" s="1" t="e">
-        <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
+      <c r="A8" t="s">
+        <v>16</v>
+      </c>
+      <c r="B8">
+        <v>300</v>
+      </c>
+      <c r="C8">
+        <v>0.75</v>
+      </c>
+      <c r="D8">
+        <v>234</v>
+      </c>
+      <c r="E8">
+        <v>277</v>
+      </c>
+      <c r="F8">
+        <v>224</v>
+      </c>
+      <c r="G8" s="1">
+        <f t="shared" si="0"/>
+        <v>98000</v>
+      </c>
+      <c r="H8" s="2">
+        <v>42869</v>
+      </c>
+      <c r="I8" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="9" spans="1:10">
-      <c r="G9" s="1" t="e">
-        <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
+      <c r="A9" t="s">
+        <v>12</v>
+      </c>
+      <c r="B9">
+        <v>50</v>
+      </c>
+      <c r="C9">
+        <v>0.75</v>
+      </c>
+      <c r="D9">
+        <v>45</v>
+      </c>
+      <c r="E9">
+        <v>59</v>
+      </c>
+      <c r="F9">
+        <v>69</v>
+      </c>
+      <c r="G9" s="1">
+        <f t="shared" si="0"/>
+        <v>3844.4444444444443</v>
+      </c>
+      <c r="H9" s="2">
+        <v>42869</v>
+      </c>
+      <c r="I9" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="10" spans="1:10">
-      <c r="G10" s="1" t="e">
-        <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
+      <c r="A10" t="s">
+        <v>2</v>
+      </c>
+      <c r="B10">
+        <v>300</v>
+      </c>
+      <c r="C10">
+        <v>0.75</v>
+      </c>
+      <c r="D10">
+        <v>127</v>
+      </c>
+      <c r="E10">
+        <v>139</v>
+      </c>
+      <c r="F10">
+        <v>126</v>
+      </c>
+      <c r="G10" s="1">
+        <f t="shared" si="0"/>
+        <v>52266.666666666657</v>
+      </c>
+      <c r="H10" s="2">
+        <v>42869</v>
+      </c>
+      <c r="I10" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="11" spans="1:10">
+      <c r="A11" t="s">
+        <v>15</v>
+      </c>
+      <c r="B11">
+        <v>300</v>
+      </c>
+      <c r="C11">
+        <v>0.2</v>
+      </c>
+      <c r="D11" t="s">
+        <v>24</v>
+      </c>
+      <c r="E11" t="s">
+        <v>25</v>
+      </c>
+      <c r="F11" t="s">
+        <v>26</v>
+      </c>
       <c r="G11" s="1" t="e">
         <f t="shared" si="0"/>
         <v>#DIV/0!</v>
       </c>
+      <c r="H11" s="2">
+        <v>42870</v>
+      </c>
+      <c r="I11" t="s">
+        <v>34</v>
+      </c>
     </row>
     <row r="12" spans="1:10">
+      <c r="A12" t="s">
+        <v>27</v>
+      </c>
+      <c r="B12">
+        <v>300</v>
+      </c>
+      <c r="C12">
+        <v>0.2</v>
+      </c>
+      <c r="D12" t="s">
+        <v>28</v>
+      </c>
+      <c r="E12" t="s">
+        <v>29</v>
+      </c>
+      <c r="F12" t="s">
+        <v>30</v>
+      </c>
       <c r="G12" s="1" t="e">
         <f t="shared" si="0"/>
         <v>#DIV/0!</v>
       </c>
+      <c r="H12" s="2">
+        <v>42870</v>
+      </c>
+      <c r="I12" t="s">
+        <v>34</v>
+      </c>
     </row>
     <row r="13" spans="1:10">
+      <c r="A13" t="s">
+        <v>16</v>
+      </c>
+      <c r="B13">
+        <v>150</v>
+      </c>
+      <c r="C13">
+        <v>0.2</v>
+      </c>
+      <c r="D13" t="s">
+        <v>31</v>
+      </c>
+      <c r="E13" t="s">
+        <v>32</v>
+      </c>
+      <c r="F13" t="s">
+        <v>33</v>
+      </c>
       <c r="G13" s="1" t="e">
         <f t="shared" si="0"/>
         <v>#DIV/0!</v>
+      </c>
+      <c r="H13" s="2">
+        <v>42870</v>
+      </c>
+      <c r="I13" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="14" spans="1:10">
@@ -667,6 +1056,9 @@
         <f t="shared" si="0"/>
         <v>#DIV/0!</v>
       </c>
+      <c r="J15" t="s">
+        <v>36</v>
+      </c>
     </row>
     <row r="16" spans="1:10">
       <c r="G16" s="1" t="e">
@@ -772,7 +1164,108 @@
     </row>
     <row r="1048576" spans="9:9">
       <c r="I1048576" t="s">
+        <v>5</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:K2"/>
+  <sheetViews>
+    <sheetView showRuler="0" workbookViewId="0">
+      <selection activeCell="J20" sqref="J20"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="1" max="1" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.5" customWidth="1"/>
+    <col min="8" max="8" width="19" customWidth="1"/>
+    <col min="9" max="10" width="18.1640625" customWidth="1"/>
+    <col min="11" max="11" width="61.6640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" s="5" customFormat="1" ht="46" customHeight="1">
+      <c r="A1" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="E1" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="F1" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="G1" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="H1" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="I1" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="J1" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="K1" s="5" t="s">
         <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11">
+      <c r="A2" s="2">
+        <v>42870</v>
+      </c>
+      <c r="B2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2">
+        <v>300</v>
+      </c>
+      <c r="D2">
+        <v>0.2</v>
+      </c>
+      <c r="E2">
+        <v>51</v>
+      </c>
+      <c r="F2">
+        <v>71</v>
+      </c>
+      <c r="G2">
+        <v>67</v>
+      </c>
+      <c r="H2" s="1">
+        <f t="shared" ref="H2" si="0">(AVERAGE(E2:G2)/D2)*C2</f>
+        <v>94500</v>
+      </c>
+      <c r="I2" s="1">
+        <f>'Larval collection counts'!G2+'Larval collection counts'!G5+'Larval Counts - rearing bucket'!G5</f>
+        <v>114200</v>
+      </c>
+      <c r="J2" s="6">
+        <f>H2/I2</f>
+        <v>0.82749562171628721</v>
+      </c>
+      <c r="K2" t="s">
+        <v>35</v>
       </c>
     </row>
   </sheetData>

</xml_diff>